<commit_message>
updated covid 19 vaccine brand name mapping
added COVVALNEVA, COVNOVAVAX
</commit_message>
<xml_diff>
--- a/reference/CPRD Gold.xlsx
+++ b/reference/CPRD Gold.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\ETL-CDMBuilder\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CE8658-BC79-48E6-9ECC-B5E538F48EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC89728-4EBB-47CE-9050-E1D063A4BA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25635" yWindow="3690" windowWidth="25140" windowHeight="11295" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cdm_gold_202201" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,9 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
     <sheet name="cdm_gold_202201_new" sheetId="4" r:id="rId4"/>
     <sheet name="cdm_gold_202301" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="7" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cdm_gold_202201!$A$1:$G$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sheet2!$A$1:$B$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="103">
   <si>
     <t>Table Name</t>
   </si>
@@ -295,63 +292,9 @@
     <t>For person_id = 410132</t>
   </si>
   <si>
-    <t>Review PK and indexes</t>
-  </si>
-  <si>
-    <t>patient</t>
-  </si>
-  <si>
-    <t>practice</t>
-  </si>
-  <si>
-    <t>staff</t>
-  </si>
-  <si>
-    <t>clinical</t>
-  </si>
-  <si>
-    <t>additional</t>
-  </si>
-  <si>
-    <t>consultation</t>
-  </si>
-  <si>
-    <t>immunisation</t>
-  </si>
-  <si>
-    <t>referral</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>therapy</t>
-  </si>
-  <si>
-    <t>2020_07</t>
-  </si>
-  <si>
-    <t>2022_07</t>
-  </si>
-  <si>
-    <t>Drug_era</t>
-  </si>
-  <si>
-    <t>2022_01</t>
-  </si>
-  <si>
-    <t>CVX</t>
-  </si>
-  <si>
     <t>Map All Death</t>
   </si>
   <si>
-    <t>Cdm Object</t>
-  </si>
-  <si>
-    <t>withinTheObservationPeriod</t>
-  </si>
-  <si>
     <t>1. Death</t>
   </si>
   <si>
@@ -383,13 +326,37 @@
   </si>
   <si>
     <t>withinTheObservationPeriod flag exists</t>
+  </si>
+  <si>
+    <t>Original ETLBuilder Logic</t>
+  </si>
+  <si>
+    <t>New Logic</t>
+  </si>
+  <si>
+    <t>Cdm Table</t>
+  </si>
+  <si>
+    <t>Map with consideration of ObservationPeriod</t>
+  </si>
+  <si>
+    <t>withinTheObservationPeriod flag</t>
+  </si>
+  <si>
+    <t>WithinTheObservationPeriod in App.config</t>
+  </si>
+  <si>
+    <t>Controlled by the parameter WithinTheObservationPeriod in App.config</t>
+  </si>
+  <si>
+    <t>Reject Death if coming before the start of observation period and after 3 months from the end of it</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -538,20 +505,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -761,8 +735,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDFDFDF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E2F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -929,6 +915,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -974,7 +997,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -989,30 +1012,71 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1862,7 +1926,7 @@
         <v>16958587</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="13" t="b">
+      <c r="D18" s="22" t="b">
         <f>(B18+B19)=C4</f>
         <v>1</v>
       </c>
@@ -1875,7 +1939,7 @@
         <v>3822372</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="13"/>
+      <c r="D19" s="22"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2403,8 +2467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8524FF28-3A11-4EBE-9E83-632FCB135758}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2503,7 +2567,7 @@
         <v>50</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>51</v>
@@ -2599,7 +2663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29CEFE6-8739-42DF-8663-0A1BDE438756}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -2769,7 +2833,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="22" t="s">
         <v>46</v>
       </c>
       <c r="B17" t="s">
@@ -2780,7 +2844,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="22"/>
       <c r="B18" t="s">
         <v>58</v>
       </c>
@@ -2789,7 +2853,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="A19" s="22"/>
       <c r="B19" t="s">
         <v>59</v>
       </c>
@@ -2805,7 +2869,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="22" t="s">
         <v>63</v>
       </c>
       <c r="B22" t="s">
@@ -2816,46 +2880,46 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
+      <c r="A23" s="22"/>
       <c r="B23" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
+      <c r="A24" s="22"/>
       <c r="B24" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
+      <c r="A25" s="22"/>
       <c r="B25" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
+      <c r="A26" s="22"/>
       <c r="B26" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14" t="s">
+      <c r="C28" s="23"/>
+      <c r="D28" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14" t="s">
+      <c r="E28" s="23"/>
+      <c r="F28" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14" t="s">
+      <c r="G28" s="23"/>
+      <c r="H28" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="I28" s="14"/>
+      <c r="I28" s="23"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -3174,279 +3238,198 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97ACBCA-5FCB-4E19-90CD-E63D4EDF1841}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12"/>
+      <c r="B1" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="27"/>
+    </row>
+    <row r="2" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="29"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="32"/>
+      <c r="E6" s="29"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="32"/>
+      <c r="E7" s="29"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="29"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="32"/>
+      <c r="E9" s="29"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="29"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
         <v>93</v>
       </c>
+      <c r="B12" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="30"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E609D6-CED1-4563-9069-3E8725544994}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2">
-        <v>848754959</v>
-      </c>
-      <c r="C2">
-        <v>788920159</v>
-      </c>
-      <c r="D2">
-        <v>797675024</v>
-      </c>
-      <c r="E2" s="12">
-        <f>(B2-C2)</f>
-        <v>59834800</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3">
-        <v>195</v>
-      </c>
-      <c r="C3">
-        <v>231</v>
-      </c>
-      <c r="D3">
-        <v>251</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF642C6-9286-4215-A492-E6C51B9FE602}">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="E4:E12"/>
+    <mergeCell ref="D3:D12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>